<commit_message>
Auto-run .py code. Re-runs for the presentation. 26-May-2023
</commit_message>
<xml_diff>
--- a/analysis/Analysis_Experiments_V11_22-May-2023.xlsx
+++ b/analysis/Analysis_Experiments_V11_22-May-2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\results\20-May-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0253D49B-BAFE-4850-B0C1-B2ECAABD8C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFBB7BF-86DA-4BAF-923C-005C8A18036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="521" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="521" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simulated Env." sheetId="12" r:id="rId1"/>
@@ -3102,30 +3102,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FF1CF8-24B8-4488-B39C-375B998FA012}">
   <dimension ref="A2:Y89"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="38" customWidth="1"/>
-    <col min="6" max="15" width="9.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="1" customWidth="1"/>
-    <col min="17" max="18" width="9.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" customWidth="1"/>
-    <col min="20" max="20" width="8.140625" customWidth="1"/>
-    <col min="21" max="21" width="30.85546875" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="8.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="38" customWidth="1"/>
+    <col min="6" max="15" width="9.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="1" customWidth="1"/>
+    <col min="17" max="18" width="9.44140625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" customWidth="1"/>
+    <col min="20" max="20" width="8.109375" customWidth="1"/>
+    <col min="21" max="21" width="30.88671875" customWidth="1"/>
+    <col min="22" max="22" width="8.109375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:25" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:25" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="25" t="s">
         <v>99</v>
       </c>
@@ -3133,14 +3133,14 @@
         <v>45064</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="P3" s="104" t="s">
         <v>125</v>
       </c>
       <c r="Q3" s="104"/>
       <c r="R3" s="104"/>
     </row>
-    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4" s="63" t="s">
         <v>5</v>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="Y4" s="19"/>
     </row>
-    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5" s="65"/>
       <c r="C5" s="66"/>
@@ -3242,7 +3242,7 @@
       <c r="X5" s="62"/>
       <c r="Y5" s="19"/>
     </row>
-    <row r="6" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>17</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>71</v>
       </c>
@@ -3330,7 +3330,7 @@
       <c r="U7" s="3"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>95</v>
@@ -3385,7 +3385,7 @@
       <c r="W8" s="8"/>
       <c r="X8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>119</v>
       </c>
@@ -3499,7 +3499,7 @@
       <c r="W11" s="50"/>
       <c r="X11" s="51"/>
     </row>
-    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>18</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>1.234</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>1.234</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
@@ -3694,7 +3694,7 @@
       <c r="W15" s="50"/>
       <c r="X15" s="51"/>
     </row>
-    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>46</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>119</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>19</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="19" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>71</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="20" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="W21"/>
     </row>
-    <row r="22" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
@@ -4031,7 +4031,7 @@
       </c>
       <c r="W22"/>
     </row>
-    <row r="23" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
         <v>119</v>
       </c>
@@ -4046,196 +4046,196 @@
       <c r="V23"/>
       <c r="W23"/>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C24" s="6"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C25" s="6"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C26" s="6"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C27" s="6"/>
       <c r="S27" s="1"/>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C28" s="6"/>
       <c r="S28" s="1"/>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C29" s="6"/>
       <c r="S29" s="1"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C30" s="6"/>
       <c r="S30" s="1"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C31" s="6"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C32" s="6"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C33" s="6"/>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C34" s="6"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C35" s="6"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C36" s="6"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C37" s="6"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C38" s="6"/>
       <c r="S38" s="1"/>
     </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C39" s="6"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C40" s="6"/>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C41" s="6"/>
       <c r="S41" s="1"/>
     </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C42" s="6"/>
       <c r="S42" s="1"/>
     </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C43" s="6"/>
       <c r="S43" s="1"/>
     </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C44" s="6"/>
       <c r="S44" s="1"/>
     </row>
-    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C45" s="6"/>
       <c r="S45" s="1"/>
     </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C46" s="6"/>
       <c r="S46" s="1"/>
     </row>
-    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C47" s="6"/>
       <c r="S47" s="1"/>
     </row>
-    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C48" s="6"/>
       <c r="S48" s="1"/>
     </row>
-    <row r="49" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C49" s="6"/>
       <c r="S49" s="1"/>
     </row>
-    <row r="50" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C50" s="6"/>
       <c r="S50" s="1"/>
     </row>
-    <row r="51" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C51" s="6"/>
       <c r="S51" s="1"/>
     </row>
-    <row r="52" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C52" s="6"/>
       <c r="S52" s="1"/>
     </row>
-    <row r="53" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C53" s="6"/>
       <c r="S53" s="1"/>
     </row>
-    <row r="54" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C54" s="6"/>
       <c r="S54" s="1"/>
     </row>
-    <row r="55" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C55" s="6"/>
       <c r="S55" s="1"/>
     </row>
-    <row r="56" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C56" s="6"/>
       <c r="S56" s="1"/>
     </row>
-    <row r="57" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C57" s="6"/>
       <c r="S57" s="1"/>
     </row>
-    <row r="58" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C58" s="6"/>
       <c r="S58" s="1"/>
     </row>
-    <row r="59" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C59" s="6"/>
       <c r="S59" s="1"/>
     </row>
-    <row r="60" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C60" s="6"/>
       <c r="S60" s="1"/>
     </row>
-    <row r="61" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C61" s="6"/>
       <c r="S61" s="1"/>
     </row>
-    <row r="62" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C62" s="6"/>
       <c r="S62" s="1"/>
     </row>
-    <row r="63" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C63" s="6"/>
       <c r="S63" s="1"/>
     </row>
-    <row r="64" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:19" x14ac:dyDescent="0.3">
       <c r="C64" s="6"/>
       <c r="S64" s="1"/>
     </row>
-    <row r="65" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C65" s="6"/>
       <c r="S65" s="1"/>
     </row>
-    <row r="66" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C66" s="6"/>
       <c r="S66" s="1"/>
     </row>
-    <row r="67" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:19" x14ac:dyDescent="0.3">
       <c r="C67" s="6"/>
       <c r="S67" s="1"/>
     </row>
-    <row r="68" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:19" x14ac:dyDescent="0.3">
       <c r="S68" s="1"/>
     </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:19" x14ac:dyDescent="0.3">
       <c r="S69" s="1"/>
     </row>
-    <row r="70" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:19" x14ac:dyDescent="0.3">
       <c r="E70" s="34"/>
       <c r="S70" s="1"/>
     </row>
-    <row r="71" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:19" x14ac:dyDescent="0.3">
       <c r="S71" s="1"/>
     </row>
-    <row r="72" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B72" s="21" t="s">
         <v>35</v>
       </c>
@@ -4256,7 +4256,7 @@
       <c r="Q72" s="24"/>
       <c r="R72" s="42"/>
     </row>
-    <row r="73" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
@@ -4275,12 +4275,12 @@
       <c r="Q73"/>
       <c r="R73"/>
     </row>
-    <row r="88" spans="21:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="21:23" x14ac:dyDescent="0.3">
       <c r="U88" s="3"/>
       <c r="V88"/>
       <c r="W88"/>
     </row>
-    <row r="89" spans="21:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="21:23" x14ac:dyDescent="0.3">
       <c r="V89"/>
       <c r="W89"/>
     </row>
@@ -4306,31 +4306,31 @@
   </sheetPr>
   <dimension ref="A2:AD83"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="38" customWidth="1"/>
-    <col min="8" max="20" width="9.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" customWidth="1"/>
-    <col min="23" max="23" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5703125" customWidth="1"/>
-    <col min="28" max="30" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="38" customWidth="1"/>
+    <col min="8" max="20" width="9.44140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" customWidth="1"/>
+    <col min="22" max="22" width="8.109375" customWidth="1"/>
+    <col min="23" max="23" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.109375" style="3" customWidth="1"/>
+    <col min="25" max="25" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5546875" customWidth="1"/>
+    <col min="28" max="30" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="25" t="s">
         <v>100</v>
       </c>
@@ -4338,8 +4338,8 @@
         <v>45064</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:27" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:27" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
         <v>73</v>
       </c>
@@ -4399,7 +4399,7 @@
       </c>
       <c r="AA4" s="19"/>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="78">
         <v>0.12</v>
       </c>
@@ -4451,7 +4451,7 @@
       <c r="Z5" s="19"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>208</v>
       </c>
@@ -4490,7 +4490,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>71</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>95</v>
@@ -4633,7 +4633,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>0.47799999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
@@ -4753,7 +4753,7 @@
       <c r="Z10" s="51"/>
       <c r="AA10" s="51"/>
     </row>
-    <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>119</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="14" t="s">
         <v>75</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>1.234</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
@@ -4874,7 +4874,7 @@
         <v>0.86967899999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>95</v>
       </c>
@@ -4931,7 +4931,7 @@
       </c>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
@@ -4995,7 +4995,7 @@
       <c r="Z15" s="51"/>
       <c r="AA15" s="51"/>
     </row>
-    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>46</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>119</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="14" t="s">
         <v>76</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
@@ -5243,7 +5243,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="Y21"/>
     </row>
-    <row r="22" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
@@ -5372,7 +5372,7 @@
       </c>
       <c r="Y22"/>
     </row>
-    <row r="23" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="2" t="s">
         <v>119</v>
       </c>
@@ -5394,7 +5394,7 @@
       </c>
       <c r="Y23"/>
     </row>
-    <row r="24" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
         <v>78</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="78">
         <v>9.8000000000000004E-2</v>
       </c>
@@ -5488,7 +5488,7 @@
       <c r="T25" s="74"/>
       <c r="U25" s="69"/>
     </row>
-    <row r="26" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
         <v>199</v>
       </c>
@@ -5516,7 +5516,7 @@
       <c r="X26"/>
       <c r="Y26"/>
     </row>
-    <row r="27" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>6</v>
       </c>
@@ -5577,7 +5577,7 @@
       <c r="X27"/>
       <c r="Y27"/>
     </row>
-    <row r="28" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
         <v>95</v>
@@ -5636,7 +5636,7 @@
       <c r="X28"/>
       <c r="Y28"/>
     </row>
-    <row r="29" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
         <v>72</v>
       </c>
@@ -5694,7 +5694,7 @@
       <c r="X29"/>
       <c r="Y29"/>
     </row>
-    <row r="30" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
@@ -5753,7 +5753,7 @@
       <c r="X30"/>
       <c r="Y30"/>
     </row>
-    <row r="31" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
         <v>119</v>
       </c>
@@ -5765,7 +5765,7 @@
       <c r="X31"/>
       <c r="Y31"/>
     </row>
-    <row r="32" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="14" t="s">
         <v>79</v>
       </c>
@@ -5797,7 +5797,7 @@
       <c r="AC32" s="1"/>
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
@@ -5865,7 +5865,7 @@
       <c r="AC33" s="1"/>
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="2" t="s">
         <v>95</v>
       </c>
@@ -5930,7 +5930,7 @@
       <c r="AC34" s="1"/>
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="2" t="s">
         <v>72</v>
       </c>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="2" t="s">
         <v>46</v>
       </c>
@@ -6045,7 +6045,7 @@
       </c>
       <c r="U36" s="1"/>
     </row>
-    <row r="37" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="2" t="s">
         <v>119</v>
       </c>
@@ -6061,7 +6061,7 @@
       <c r="T37" s="7"/>
       <c r="U37" s="1"/>
     </row>
-    <row r="38" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="14" t="s">
         <v>80</v>
       </c>
@@ -6087,7 +6087,7 @@
       </c>
       <c r="U38" s="16"/>
     </row>
-    <row r="39" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="3" t="s">
         <v>6</v>
       </c>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="U39" s="1"/>
     </row>
-    <row r="40" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
         <v>95</v>
       </c>
@@ -6205,7 +6205,7 @@
       </c>
       <c r="U40" s="1"/>
     </row>
-    <row r="41" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C41" s="2" t="s">
         <v>72</v>
       </c>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="U41" s="1"/>
     </row>
-    <row r="42" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="2" t="s">
         <v>46</v>
       </c>
@@ -6320,7 +6320,7 @@
       </c>
       <c r="U42" s="1"/>
     </row>
-    <row r="43" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
         <v>119</v>
       </c>
@@ -6345,10 +6345,10 @@
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U44" s="1"/>
     </row>
-    <row r="45" spans="1:30" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" ht="25.8" x14ac:dyDescent="0.3">
       <c r="A45" s="77" t="s">
         <v>81</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="78">
         <v>0.13</v>
       </c>
@@ -6442,7 +6442,7 @@
       <c r="T46" s="74"/>
       <c r="U46" s="69"/>
     </row>
-    <row r="47" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="14" t="s">
         <v>201</v>
       </c>
@@ -6466,7 +6466,7 @@
       <c r="T47" s="16"/>
       <c r="U47" s="16"/>
     </row>
-    <row r="48" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
         <v>10</v>
       </c>
@@ -6527,7 +6527,7 @@
       </c>
       <c r="U48" s="1"/>
     </row>
-    <row r="49" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
         <v>61</v>
@@ -6585,7 +6585,7 @@
       </c>
       <c r="U49" s="1"/>
     </row>
-    <row r="50" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="2" t="s">
         <v>72</v>
       </c>
@@ -6642,7 +6642,7 @@
       </c>
       <c r="U50" s="1"/>
     </row>
-    <row r="51" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="2" t="s">
         <v>46</v>
       </c>
@@ -6700,7 +6700,7 @@
       </c>
       <c r="U51" s="1"/>
     </row>
-    <row r="52" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C52" s="2" t="s">
         <v>119</v>
       </c>
@@ -6710,7 +6710,7 @@
       <c r="E52" s="47"/>
       <c r="F52" s="47"/>
     </row>
-    <row r="53" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="14" t="s">
         <v>83</v>
       </c>
@@ -6734,7 +6734,7 @@
       <c r="T53" s="16"/>
       <c r="U53" s="16"/>
     </row>
-    <row r="54" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="3" t="s">
         <v>10</v>
       </c>
@@ -6795,7 +6795,7 @@
       </c>
       <c r="U54" s="1"/>
     </row>
-    <row r="55" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C55" s="2" t="s">
         <v>61</v>
       </c>
@@ -6852,7 +6852,7 @@
       </c>
       <c r="U55" s="1"/>
     </row>
-    <row r="56" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
         <v>72</v>
       </c>
@@ -6909,7 +6909,7 @@
       </c>
       <c r="U56" s="1"/>
     </row>
-    <row r="57" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="2" t="s">
         <v>46</v>
       </c>
@@ -6967,7 +6967,7 @@
       </c>
       <c r="U57" s="1"/>
     </row>
-    <row r="58" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C58" s="2" t="s">
         <v>119</v>
       </c>
@@ -6983,7 +6983,7 @@
       <c r="T58" s="7"/>
       <c r="U58" s="1"/>
     </row>
-    <row r="59" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="14" t="s">
         <v>84</v>
       </c>
@@ -7007,7 +7007,7 @@
       <c r="T59" s="16"/>
       <c r="U59" s="16"/>
     </row>
-    <row r="60" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
         <v>10</v>
       </c>
@@ -7068,7 +7068,7 @@
       </c>
       <c r="U60" s="1"/>
     </row>
-    <row r="61" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="2" t="s">
         <v>61</v>
       </c>
@@ -7125,7 +7125,7 @@
       </c>
       <c r="U61" s="1"/>
     </row>
-    <row r="62" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="2" t="s">
         <v>72</v>
       </c>
@@ -7182,7 +7182,7 @@
       </c>
       <c r="U62" s="1"/>
     </row>
-    <row r="63" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="2" t="s">
         <v>46</v>
       </c>
@@ -7240,7 +7240,7 @@
       </c>
       <c r="U63" s="41"/>
     </row>
-    <row r="64" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C64" s="2" t="s">
         <v>90</v>
       </c>
@@ -7265,14 +7265,14 @@
       <c r="T64" s="75"/>
       <c r="U64" s="34"/>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C65" s="6"/>
       <c r="U65" s="1"/>
     </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.3">
       <c r="U66" s="1"/>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
@@ -7293,32 +7293,32 @@
       <c r="S67"/>
       <c r="T67"/>
     </row>
-    <row r="82" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="23:25" x14ac:dyDescent="0.3">
       <c r="W82" s="3"/>
       <c r="X82"/>
       <c r="Y82"/>
     </row>
-    <row r="83" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="23:25" x14ac:dyDescent="0.3">
       <c r="X83"/>
       <c r="Y83"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P24:Q24"/>
     <mergeCell ref="H45:I45"/>
     <mergeCell ref="J45:K45"/>
     <mergeCell ref="L45:M45"/>
     <mergeCell ref="N45:O45"/>
     <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="landscape" r:id="rId1"/>
@@ -7332,31 +7332,31 @@
   </sheetPr>
   <dimension ref="A2:AD113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="38" customWidth="1"/>
-    <col min="8" max="20" width="9.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="17.28515625" customWidth="1"/>
-    <col min="22" max="22" width="8.140625" customWidth="1"/>
-    <col min="23" max="23" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.5703125" customWidth="1"/>
-    <col min="28" max="30" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="38" customWidth="1"/>
+    <col min="8" max="20" width="9.44140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" customWidth="1"/>
+    <col min="22" max="22" width="8.109375" customWidth="1"/>
+    <col min="23" max="23" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.109375" style="3" customWidth="1"/>
+    <col min="25" max="25" width="6.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5546875" customWidth="1"/>
+    <col min="28" max="30" width="8.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="25" t="s">
         <v>102</v>
       </c>
@@ -7364,8 +7364,8 @@
         <v>45065</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:27" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:27" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
         <v>73</v>
       </c>
@@ -7425,7 +7425,7 @@
       </c>
       <c r="AA4" s="19"/>
     </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="78">
         <v>0.12</v>
       </c>
@@ -7477,7 +7477,7 @@
       <c r="Z5" s="19"/>
       <c r="AA5" s="19"/>
     </row>
-    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
         <v>74</v>
       </c>
@@ -7518,7 +7518,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>213</v>
       </c>
@@ -7593,7 +7593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>95</v>
@@ -7666,7 +7666,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>72</v>
       </c>
@@ -7723,7 +7723,7 @@
       </c>
       <c r="U9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
@@ -7788,7 +7788,7 @@
       <c r="Z10" s="51"/>
       <c r="AA10" s="51"/>
     </row>
-    <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>119</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
@@ -7845,7 +7845,7 @@
         <v>1.234</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>212</v>
       </c>
@@ -7912,7 +7912,7 @@
         <v>0.86967899999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>95</v>
@@ -7970,7 +7970,7 @@
       </c>
       <c r="U14" s="3"/>
     </row>
-    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
@@ -8034,7 +8034,7 @@
       <c r="Z15" s="51"/>
       <c r="AA15" s="51"/>
     </row>
-    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>46</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
         <v>119</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -8150,7 +8150,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="98" t="s">
         <v>214</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="2" t="s">
         <v>72</v>
       </c>
@@ -8343,7 +8343,7 @@
       </c>
       <c r="Y21"/>
     </row>
-    <row r="22" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
@@ -8407,7 +8407,7 @@
       </c>
       <c r="Y22"/>
     </row>
-    <row r="23" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
         <v>119</v>
       </c>
@@ -8433,7 +8433,7 @@
       </c>
       <c r="Y23"/>
     </row>
-    <row r="24" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -8455,7 +8455,7 @@
       <c r="U24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>75</v>
       </c>
@@ -8479,7 +8479,7 @@
       <c r="T25" s="16"/>
       <c r="U25" s="91"/>
     </row>
-    <row r="26" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
@@ -8540,7 +8540,7 @@
       </c>
       <c r="U26" s="41"/>
     </row>
-    <row r="27" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="2" t="s">
         <v>95</v>
       </c>
@@ -8597,7 +8597,7 @@
       </c>
       <c r="U27" s="41"/>
     </row>
-    <row r="28" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="2" t="s">
         <v>72</v>
       </c>
@@ -8654,7 +8654,7 @@
       </c>
       <c r="U28" s="41"/>
     </row>
-    <row r="29" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
         <v>46</v>
       </c>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="U29" s="41"/>
     </row>
-    <row r="30" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="2" t="s">
         <v>119</v>
       </c>
@@ -8730,7 +8730,7 @@
       <c r="Z30" s="3"/>
       <c r="AA30" s="3"/>
     </row>
-    <row r="31" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
         <v>76</v>
       </c>
@@ -8757,7 +8757,7 @@
       <c r="Z31" s="3"/>
       <c r="AA31" s="3"/>
     </row>
-    <row r="32" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
@@ -8778,7 +8778,7 @@
       <c r="Z32" s="3"/>
       <c r="AA32" s="3"/>
     </row>
-    <row r="33" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="2" t="s">
         <v>95</v>
       </c>
@@ -8795,7 +8795,7 @@
       <c r="Z33" s="3"/>
       <c r="AA33" s="3"/>
     </row>
-    <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="2" t="s">
         <v>72</v>
       </c>
@@ -8812,7 +8812,7 @@
       <c r="Z34" s="3"/>
       <c r="AA34" s="3"/>
     </row>
-    <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="2" t="s">
         <v>46</v>
       </c>
@@ -8841,7 +8841,7 @@
       <c r="W35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="2" t="s">
         <v>119</v>
       </c>
@@ -8858,7 +8858,7 @@
       <c r="W36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D37" s="47"/>
       <c r="E37" s="47"/>
       <c r="F37" s="47"/>
@@ -8870,7 +8870,7 @@
       <c r="W37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="77" t="s">
         <v>78</v>
       </c>
@@ -8919,7 +8919,7 @@
       <c r="W38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="78">
         <v>9.8000000000000004E-2</v>
       </c>
@@ -8966,7 +8966,7 @@
       <c r="T39" s="74"/>
       <c r="U39" s="90"/>
     </row>
-    <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="95"/>
       <c r="B40" s="14" t="s">
         <v>134</v>
@@ -8991,7 +8991,7 @@
       <c r="T40" s="16"/>
       <c r="U40" s="91"/>
     </row>
-    <row r="41" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="3" t="s">
         <v>6</v>
       </c>
@@ -9051,7 +9051,7 @@
       </c>
       <c r="U41" s="3"/>
     </row>
-    <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
         <v>213</v>
       </c>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="U42" s="3"/>
     </row>
-    <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
         <v>72</v>
       </c>
@@ -9168,7 +9168,7 @@
       </c>
       <c r="U43" s="3"/>
     </row>
-    <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C44" s="2" t="s">
         <v>46</v>
       </c>
@@ -9226,7 +9226,7 @@
       </c>
       <c r="U44" s="3"/>
     </row>
-    <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C45" s="2" t="s">
         <v>119</v>
       </c>
@@ -9237,7 +9237,7 @@
       <c r="F45" s="47"/>
       <c r="U45" s="3"/>
     </row>
-    <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D46" s="47"/>
       <c r="E46" s="47"/>
       <c r="F46" s="47"/>
@@ -9246,7 +9246,7 @@
       </c>
       <c r="U46" s="3"/>
     </row>
-    <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="3" t="s">
         <v>6</v>
       </c>
@@ -9306,7 +9306,7 @@
       </c>
       <c r="U47" s="3"/>
     </row>
-    <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="3" t="s">
         <v>212</v>
       </c>
@@ -9366,7 +9366,7 @@
       </c>
       <c r="U48" s="3"/>
     </row>
-    <row r="49" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C49" s="2" t="s">
         <v>72</v>
       </c>
@@ -9423,7 +9423,7 @@
       </c>
       <c r="U49" s="3"/>
     </row>
-    <row r="50" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C50" s="2" t="s">
         <v>46</v>
       </c>
@@ -9481,7 +9481,7 @@
       </c>
       <c r="U50" s="3"/>
     </row>
-    <row r="51" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C51" s="2" t="s">
         <v>119</v>
       </c>
@@ -9492,7 +9492,7 @@
       <c r="F51" s="47"/>
       <c r="U51" s="3"/>
     </row>
-    <row r="52" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="14" t="s">
         <v>79</v>
       </c>
@@ -9518,7 +9518,7 @@
       </c>
       <c r="U52" s="91"/>
     </row>
-    <row r="53" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="3" t="s">
         <v>6</v>
       </c>
@@ -9579,7 +9579,7 @@
       </c>
       <c r="U53" s="41"/>
     </row>
-    <row r="54" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C54" s="2" t="s">
         <v>95</v>
       </c>
@@ -9636,7 +9636,7 @@
       </c>
       <c r="U54" s="41"/>
     </row>
-    <row r="55" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C55" s="2" t="s">
         <v>72</v>
       </c>
@@ -9693,7 +9693,7 @@
       </c>
       <c r="U55" s="41"/>
     </row>
-    <row r="56" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C56" s="2" t="s">
         <v>46</v>
       </c>
@@ -9752,7 +9752,7 @@
       <c r="X56"/>
       <c r="Y56"/>
     </row>
-    <row r="57" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C57" s="2" t="s">
         <v>119</v>
       </c>
@@ -9770,7 +9770,7 @@
       <c r="X57"/>
       <c r="Y57"/>
     </row>
-    <row r="58" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="14" t="s">
         <v>80</v>
       </c>
@@ -9796,7 +9796,7 @@
       <c r="X58"/>
       <c r="Y58"/>
     </row>
-    <row r="59" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
         <v>6</v>
       </c>
@@ -9815,7 +9815,7 @@
       <c r="X59"/>
       <c r="Y59"/>
     </row>
-    <row r="60" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C60" s="2" t="s">
         <v>95</v>
       </c>
@@ -9832,7 +9832,7 @@
       <c r="X60"/>
       <c r="Y60"/>
     </row>
-    <row r="61" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C61" s="2" t="s">
         <v>72</v>
       </c>
@@ -9848,7 +9848,7 @@
       <c r="X61"/>
       <c r="Y61"/>
     </row>
-    <row r="62" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="2" t="s">
         <v>46</v>
       </c>
@@ -9883,7 +9883,7 @@
       <c r="AC62" s="1"/>
       <c r="AD62" s="1"/>
     </row>
-    <row r="63" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:30" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="2" t="s">
         <v>119</v>
       </c>
@@ -9916,7 +9916,7 @@
       <c r="AC63" s="1"/>
       <c r="AD63" s="1"/>
     </row>
-    <row r="64" spans="2:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:30" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U64" s="41"/>
       <c r="W64" s="1"/>
       <c r="X64" s="41"/>
@@ -9927,7 +9927,7 @@
       <c r="AC64" s="1"/>
       <c r="AD64" s="1"/>
     </row>
-    <row r="65" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="77" t="s">
         <v>81</v>
       </c>
@@ -9974,7 +9974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="78">
         <v>0.13</v>
       </c>
@@ -10021,7 +10021,7 @@
       <c r="T66" s="74"/>
       <c r="U66" s="90"/>
     </row>
-    <row r="67" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="95"/>
       <c r="B67" s="14" t="s">
         <v>82</v>
@@ -10046,7 +10046,7 @@
       <c r="T67" s="16"/>
       <c r="U67" s="91"/>
     </row>
-    <row r="68" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
         <v>10</v>
       </c>
@@ -10107,7 +10107,7 @@
       </c>
       <c r="U68" s="41"/>
     </row>
-    <row r="69" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
         <v>61</v>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="U69" s="41"/>
     </row>
-    <row r="70" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="2" t="s">
         <v>72</v>
       </c>
@@ -10222,7 +10222,7 @@
       </c>
       <c r="U70" s="41"/>
     </row>
-    <row r="71" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="2" t="s">
         <v>46</v>
       </c>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="U71" s="41"/>
     </row>
-    <row r="72" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="2" t="s">
         <v>119</v>
       </c>
@@ -10290,7 +10290,7 @@
       <c r="F72" s="94"/>
       <c r="U72" s="3"/>
     </row>
-    <row r="73" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="14" t="s">
         <v>83</v>
       </c>
@@ -10316,7 +10316,7 @@
       </c>
       <c r="U73" s="91"/>
     </row>
-    <row r="74" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="3" t="s">
         <v>10</v>
       </c>
@@ -10377,7 +10377,7 @@
       </c>
       <c r="U74" s="41"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C75" s="2" t="s">
         <v>61</v>
       </c>
@@ -10434,7 +10434,7 @@
       </c>
       <c r="U75" s="41"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C76" s="2" t="s">
         <v>72</v>
       </c>
@@ -10491,7 +10491,7 @@
       </c>
       <c r="U76" s="41"/>
     </row>
-    <row r="77" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="2" t="s">
         <v>46</v>
       </c>
@@ -10548,7 +10548,7 @@
       </c>
       <c r="U77" s="41"/>
     </row>
-    <row r="78" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="2" t="s">
         <v>119</v>
       </c>
@@ -10564,7 +10564,7 @@
       <c r="T78" s="7"/>
       <c r="U78" s="41"/>
     </row>
-    <row r="79" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="14" t="s">
         <v>84</v>
       </c>
@@ -10588,7 +10588,7 @@
       <c r="T79" s="16"/>
       <c r="U79" s="91"/>
     </row>
-    <row r="80" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="3" t="s">
         <v>10</v>
       </c>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="U80" s="41"/>
     </row>
-    <row r="81" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C81" s="2" t="s">
         <v>61</v>
       </c>
@@ -10623,7 +10623,7 @@
       <c r="S81" s="7"/>
       <c r="U81" s="41"/>
     </row>
-    <row r="82" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C82" s="2" t="s">
         <v>72</v>
       </c>
@@ -10637,7 +10637,7 @@
       </c>
       <c r="U82" s="41"/>
     </row>
-    <row r="83" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C83" s="2" t="s">
         <v>46</v>
       </c>
@@ -10664,7 +10664,7 @@
       <c r="T83" s="9"/>
       <c r="U83" s="93"/>
     </row>
-    <row r="84" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C84" s="2" t="s">
         <v>90</v>
       </c>
@@ -10689,14 +10689,14 @@
       <c r="T84" s="75"/>
       <c r="U84" s="34"/>
     </row>
-    <row r="85" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C85" s="6"/>
       <c r="U85" s="1"/>
     </row>
-    <row r="86" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="U86" s="1"/>
     </row>
-    <row r="87" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
@@ -10717,39 +10717,39 @@
       <c r="S87"/>
       <c r="T87"/>
     </row>
-    <row r="88" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="23:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="23:25" x14ac:dyDescent="0.3">
       <c r="W112" s="3"/>
       <c r="X112"/>
       <c r="Y112"/>
     </row>
-    <row r="113" spans="24:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="24:25" x14ac:dyDescent="0.3">
       <c r="X113"/>
       <c r="Y113"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="J65:K65"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="N65:O65"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="J38:K38"/>
     <mergeCell ref="L38:M38"/>
     <mergeCell ref="N38:O38"/>
     <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="J65:K65"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="N65:O65"/>
-    <mergeCell ref="P65:Q65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="60" orientation="landscape" r:id="rId1"/>
@@ -10765,9 +10765,9 @@
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" s="85" t="s">
         <v>138</v>
       </c>
@@ -10857,7 +10857,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>139</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>45064</v>
       </c>
@@ -11077,7 +11077,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P4" t="s">
         <v>175</v>
       </c>
@@ -11151,7 +11151,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B5" s="33" t="s">
         <v>151</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B6" s="33" t="s">
         <v>123</v>
       </c>
@@ -11377,7 +11377,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -11570,7 +11570,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -11686,7 +11686,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -11802,7 +11802,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -11918,7 +11918,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P12" t="s">
         <v>178</v>
       </c>
@@ -11992,7 +11992,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -12102,7 +12102,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>45064</v>
       </c>
@@ -12212,7 +12212,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P15" t="s">
         <v>178</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B16" s="33" t="s">
         <v>151</v>
       </c>
@@ -12399,7 +12399,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B17" s="33" t="s">
         <v>123</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -12589,7 +12589,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -12705,7 +12705,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -12821,7 +12821,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -12937,7 +12937,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -13053,7 +13053,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P23" t="s">
         <v>178</v>
       </c>
@@ -13127,7 +13127,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>139</v>
       </c>
@@ -13237,7 +13237,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A25" s="20">
         <v>45064</v>
       </c>
@@ -13347,7 +13347,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P26" t="s">
         <v>178</v>
       </c>
@@ -13421,7 +13421,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B27" s="33" t="s">
         <v>151</v>
       </c>
@@ -13534,7 +13534,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B28" s="33" t="s">
         <v>123</v>
       </c>
@@ -13647,7 +13647,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -13724,7 +13724,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -13840,7 +13840,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -13956,7 +13956,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -14072,7 +14072,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -14188,7 +14188,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P34" t="s">
         <v>188</v>
       </c>
@@ -14262,7 +14262,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P35" t="s">
         <v>189</v>
       </c>
@@ -14336,7 +14336,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P36" t="s">
         <v>190</v>
       </c>
@@ -14410,7 +14410,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P37" t="s">
         <v>178</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P38" t="s">
         <v>178</v>
       </c>
@@ -14558,7 +14558,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P39" t="s">
         <v>178</v>
       </c>
@@ -14632,7 +14632,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P40" t="s">
         <v>178</v>
       </c>
@@ -14706,7 +14706,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P41" t="s">
         <v>178</v>
       </c>
@@ -14780,7 +14780,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P42" t="s">
         <v>178</v>
       </c>
@@ -14854,7 +14854,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P43" t="s">
         <v>178</v>
       </c>
@@ -14928,7 +14928,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P44" t="s">
         <v>178</v>
       </c>
@@ -15002,7 +15002,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P45" t="s">
         <v>178</v>
       </c>
@@ -15076,7 +15076,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P46" t="s">
         <v>178</v>
       </c>
@@ -15150,7 +15150,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P47" s="88" t="s">
         <v>178</v>
       </c>
@@ -15224,7 +15224,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.3">
       <c r="P48" t="s">
         <v>191</v>
       </c>
@@ -15298,7 +15298,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="49" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P49" t="s">
         <v>192</v>
       </c>
@@ -15372,7 +15372,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P50" t="s">
         <v>193</v>
       </c>
@@ -15446,7 +15446,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P51" t="s">
         <v>194</v>
       </c>
@@ -15520,7 +15520,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P52" t="s">
         <v>178</v>
       </c>
@@ -15594,7 +15594,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P53" t="s">
         <v>178</v>
       </c>
@@ -15668,7 +15668,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P54" t="s">
         <v>178</v>
       </c>
@@ -15742,7 +15742,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="55" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P55" t="s">
         <v>178</v>
       </c>
@@ -15816,7 +15816,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="56" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P56" t="s">
         <v>178</v>
       </c>
@@ -15890,7 +15890,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="57" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P57" t="s">
         <v>178</v>
       </c>
@@ -15964,7 +15964,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P58" t="s">
         <v>178</v>
       </c>
@@ -16038,7 +16038,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P59" t="s">
         <v>178</v>
       </c>
@@ -16112,7 +16112,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P60" t="s">
         <v>178</v>
       </c>
@@ -16186,7 +16186,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="16:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="16:39" x14ac:dyDescent="0.3">
       <c r="P61" t="s">
         <v>178</v>
       </c>
@@ -16274,24 +16274,24 @@
       <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.5703125" style="3" customWidth="1"/>
-    <col min="3" max="4" width="10.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="12.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" style="3" customWidth="1"/>
+    <col min="3" max="4" width="10.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="12.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="4.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" customWidth="1"/>
-    <col min="17" max="17" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:16" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="25" t="s">
         <v>20</v>
       </c>
@@ -16299,16 +16299,16 @@
         <v>45064</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="27">
         <v>1</v>
       </c>
@@ -16325,7 +16325,7 @@
       <c r="O6" s="30"/>
       <c r="P6" s="29"/>
     </row>
-    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="27">
         <v>2</v>
       </c>
@@ -16338,7 +16338,7 @@
       <c r="L7" s="3"/>
       <c r="M7"/>
     </row>
-    <row r="8" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="27"/>
       <c r="C8" s="3"/>
       <c r="J8" s="3" t="s">
@@ -16347,7 +16347,7 @@
       <c r="L8" s="3"/>
       <c r="M8"/>
     </row>
-    <row r="9" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="27">
         <v>3</v>
       </c>
@@ -16360,7 +16360,7 @@
       <c r="L9" s="3"/>
       <c r="M9"/>
     </row>
-    <row r="10" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="27">
         <v>4</v>
       </c>
@@ -16373,7 +16373,7 @@
       <c r="L10" s="3"/>
       <c r="M10"/>
     </row>
-    <row r="11" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="27"/>
       <c r="C11" s="3"/>
       <c r="J11" s="37" t="s">
@@ -16382,14 +16382,14 @@
       <c r="L11" s="3"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="27"/>
       <c r="C12" s="3"/>
       <c r="J12" s="37"/>
       <c r="L12" s="3"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="27">
         <v>5</v>
       </c>
@@ -16458,7 +16458,7 @@
         <v>8.2570000000000005E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27">
         <v>8</v>
       </c>
@@ -16471,7 +16471,7 @@
       <c r="M16" s="33"/>
       <c r="O16" s="33"/>
     </row>
-    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="27">
         <v>9</v>
       </c>
@@ -16482,7 +16482,7 @@
       <c r="L17" s="3"/>
       <c r="M17"/>
     </row>
-    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27">
         <v>10</v>
       </c>
@@ -16499,7 +16499,7 @@
       <c r="O18" s="30"/>
       <c r="P18" s="29"/>
     </row>
-    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27">
         <v>11</v>
       </c>
@@ -16512,7 +16512,7 @@
       <c r="L19" s="3"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="27">
         <v>12</v>
       </c>
@@ -16523,7 +16523,7 @@
       <c r="L20" s="3"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="56" t="s">
         <v>105</v>
       </c>
@@ -16531,7 +16531,7 @@
       <c r="L21" s="3"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C22" s="56" t="s">
         <v>106</v>
       </c>
@@ -16539,7 +16539,7 @@
       <c r="L22" s="3"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="2:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" ht="18" x14ac:dyDescent="0.3">
       <c r="J23" s="28" t="s">
         <v>55</v>
       </c>
@@ -16550,7 +16550,7 @@
       <c r="O23" s="30"/>
       <c r="P23" s="29"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="C24" s="2" t="s">
         <v>122</v>
       </c>
@@ -16566,21 +16566,21 @@
       <c r="M24" s="33"/>
       <c r="O24" s="33"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
         <v>61</v>
       </c>
       <c r="M25" s="33"/>
       <c r="O25" s="33"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J26" t="s">
         <v>62</v>
       </c>
       <c r="M26" s="33"/>
       <c r="O26" s="33"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J27" s="34" t="s">
         <v>46</v>
       </c>
@@ -16590,7 +16590,7 @@
       <c r="M27" s="33"/>
       <c r="O27" s="33"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J28" s="34" t="s">
         <v>47</v>
       </c>
@@ -16601,7 +16601,7 @@
       <c r="M28" s="33"/>
       <c r="O28" s="33"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J29" s="34" t="s">
         <v>48</v>
       </c>
@@ -16612,7 +16612,7 @@
       <c r="M29" s="33"/>
       <c r="O29" s="33"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J30" s="34" t="s">
         <v>49</v>
       </c>
@@ -16622,7 +16622,7 @@
       <c r="M30" s="33"/>
       <c r="O30" s="33"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J31" s="34" t="s">
         <v>51</v>
       </c>
@@ -16632,7 +16632,7 @@
       <c r="M31" s="33"/>
       <c r="O31" s="33"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J32" s="34" t="s">
         <v>53</v>
       </c>
@@ -16642,7 +16642,7 @@
       <c r="M32" s="33"/>
       <c r="O32" s="33"/>
     </row>
-    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:13" x14ac:dyDescent="0.3">
       <c r="L33" s="3"/>
       <c r="M33"/>
     </row>
@@ -16664,20 +16664,20 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="57"/>
       <c r="B2" s="57" t="s">
         <v>108</v>
@@ -16690,7 +16690,7 @@
       </c>
       <c r="E2" s="57"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="57"/>
       <c r="B3" s="57" t="s">
         <v>109</v>
@@ -16703,7 +16703,7 @@
       </c>
       <c r="E3" s="57"/>
     </row>
-    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="57"/>
       <c r="B4" s="57" t="s">
         <v>114</v>
@@ -16718,7 +16718,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="57" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="57" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" s="57" t="s">
         <v>116</v>
       </c>

</xml_diff>